<commit_message>
VFDs are configurable to be have multiple vfds per suction group.
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/alerts.xlsx
+++ b/PanelCreator/src/Creator/textFiles/alerts.xlsx
@@ -432,14 +432,14 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -475,7 +475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -497,7 +497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -508,7 +508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -519,7 +519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -530,7 +530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -552,7 +552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>